<commit_message>
CORELIMS-98 - production addition of BFS #2
</commit_message>
<xml_diff>
--- a/output/block-filing-system-2/c2_exceldata.xlsx
+++ b/output/block-filing-system-2/c2_exceldata.xlsx
@@ -28,7 +28,7 @@
     <t>C2-D1-L1</t>
   </si>
   <si>
-    <t>DRW514</t>
+    <t>DRW563</t>
   </si>
   <si>
     <t>C2-D1-L2</t>
@@ -52,7 +52,7 @@
     <t>C2-D2-L1</t>
   </si>
   <si>
-    <t>DRW515</t>
+    <t>DRW564</t>
   </si>
   <si>
     <t>C2-D2-L2</t>
@@ -76,7 +76,7 @@
     <t>C2-D3-L1</t>
   </si>
   <si>
-    <t>DRW516</t>
+    <t>DRW565</t>
   </si>
   <si>
     <t>C2-D3-L2</t>
@@ -100,7 +100,7 @@
     <t>C2-D4-L1</t>
   </si>
   <si>
-    <t>DRW517</t>
+    <t>DRW566</t>
   </si>
   <si>
     <t>C2-D4-L2</t>
@@ -124,7 +124,7 @@
     <t>C2-D5-L1</t>
   </si>
   <si>
-    <t>DRW518</t>
+    <t>DRW567</t>
   </si>
   <si>
     <t>C2-D5-L2</t>
@@ -148,7 +148,7 @@
     <t>C2-D6-L1</t>
   </si>
   <si>
-    <t>DRW519</t>
+    <t>DRW568</t>
   </si>
   <si>
     <t>C2-D6-L2</t>

</xml_diff>